<commit_message>
changed names on input and variables + updated tek shares methods
</commit_message>
<xml_diff>
--- a/input/building_categories.xlsx
+++ b/input/building_categories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Brukere-felles\lfep\EBM\task_836\Energibruksmodell\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916188D9-395D-46A1-9C23-0E7E9DBE2D49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B20960-6EE9-4C08-8047-0813250CD351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30015" yWindow="4800" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9405" yWindow="1710" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -36,18 +36,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
-    <t>StorageRepairs</t>
-  </si>
-  <si>
     <t>Sports</t>
   </si>
   <si>
-    <t>Apartment</t>
-  </si>
-  <si>
-    <t>SmallHouse</t>
-  </si>
-  <si>
     <t>Kindergarten</t>
   </si>
   <si>
@@ -60,9 +51,6 @@
     <t>Office</t>
   </si>
   <si>
-    <t>Shop</t>
-  </si>
-  <si>
     <t>Hotel</t>
   </si>
   <si>
@@ -76,6 +64,18 @@
   </si>
   <si>
     <t>building_category</t>
+  </si>
+  <si>
+    <t>Apartment block</t>
+  </si>
+  <si>
+    <t>House</t>
+  </si>
+  <si>
+    <t>Retail</t>
+  </si>
+  <si>
+    <t>Storage repairs</t>
   </si>
 </sst>
 </file>
@@ -461,9 +461,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D5D47D-DC8F-4879-A7C5-EAE71647EE33}">
   <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -472,72 +470,72 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#1088 changed all strings in input .xlsx files to lower case and underscores
</commit_message>
<xml_diff>
--- a/input/building_categories.xlsx
+++ b/input/building_categories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lfep\work_space\Energibruksmodell\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79DCE3FD-F1C4-43D6-BC39-20341E08ADEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49BB44E-8133-4359-B79F-F1548565D28E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,46 +36,46 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
-    <t>Sports</t>
-  </si>
-  <si>
-    <t>Kindergarten</t>
-  </si>
-  <si>
-    <t>School</t>
-  </si>
-  <si>
-    <t>University</t>
-  </si>
-  <si>
-    <t>Office</t>
-  </si>
-  <si>
-    <t>Hotel</t>
-  </si>
-  <si>
-    <t>Hospital</t>
-  </si>
-  <si>
-    <t>Nursinghome</t>
-  </si>
-  <si>
-    <t>Culture</t>
-  </si>
-  <si>
     <t>building_category</t>
   </si>
   <si>
-    <t>Apartment block</t>
-  </si>
-  <si>
-    <t>House</t>
-  </si>
-  <si>
-    <t>Retail</t>
-  </si>
-  <si>
-    <t>Storage repairs</t>
+    <t>apartment_block</t>
+  </si>
+  <si>
+    <t>house</t>
+  </si>
+  <si>
+    <t>kindergarten</t>
+  </si>
+  <si>
+    <t>school</t>
+  </si>
+  <si>
+    <t>university</t>
+  </si>
+  <si>
+    <t>office</t>
+  </si>
+  <si>
+    <t>retail</t>
+  </si>
+  <si>
+    <t>hotel</t>
+  </si>
+  <si>
+    <t>hospital</t>
+  </si>
+  <si>
+    <t>nursinghome</t>
+  </si>
+  <si>
+    <t>culture</t>
+  </si>
+  <si>
+    <t>sports</t>
+  </si>
+  <si>
+    <t>storage_repairs</t>
   </si>
 </sst>
 </file>
@@ -460,7 +460,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D5D47D-DC8F-4879-A7C5-EAE71647EE33}">
   <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -469,67 +471,67 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>